<commit_message>
emon_GPS_Banner: Add full font with text Clean up code and fully comment
</commit_message>
<xml_diff>
--- a/emon_GPS_Banner/FontWorkbook.xlsx
+++ b/emon_GPS_Banner/FontWorkbook.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfewi\Documents\Home\emon_Suite\emon_GPS_Banner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33061570-019E-45CA-955F-EF4ABF56A0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B73881E-3003-41DE-8407-8006A6862427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D48701C4-A332-47D2-8277-888E3311C639}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Old coding" sheetId="2" r:id="rId1"/>
+    <sheet name="New coding" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,49 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
-  <si>
-    <t>Produced</t>
-  </si>
-  <si>
-    <t>Imported</t>
-  </si>
-  <si>
-    <t>Car used</t>
-  </si>
-  <si>
-    <t>Exported</t>
-  </si>
-  <si>
-    <t>Consumed</t>
-  </si>
-  <si>
-    <t>HWS</t>
-  </si>
-  <si>
-    <t>Watt hours</t>
-  </si>
-  <si>
-    <t>Last 365 days</t>
-  </si>
-  <si>
-    <t>Last 365 days value</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Scheider Produced</t>
-  </si>
-  <si>
-    <t>20-30th Mar 2023</t>
-  </si>
-  <si>
-    <t>20-30th Mar 2022</t>
-  </si>
-  <si>
-    <t>Grafana Last 365 days</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Large</t>
   </si>
@@ -106,12 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0;\-&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,52 +73,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -186,49 +115,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="5" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,190 +436,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78BBE82-D7C7-49FC-A756-EF8D4CBF3F40}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>365288</v>
-      </c>
-      <c r="C2" s="2">
-        <v>340045</v>
-      </c>
-      <c r="D2" s="2">
-        <v>10806551</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2917</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>10868</v>
-      </c>
-      <c r="C3" s="2">
-        <v>22573</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1546275</v>
-      </c>
-      <c r="E3" s="3">
-        <v>417</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1721000</v>
-      </c>
-      <c r="G3" s="9">
-        <f>((D3-F3)/F3)</f>
-        <v>-0.10152527600232424</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>103747</v>
-      </c>
-      <c r="C4" s="2">
-        <v>68223</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1956852</v>
-      </c>
-      <c r="E4" s="3">
-        <v>528</v>
-      </c>
-      <c r="F4" s="8">
-        <v>2233000</v>
-      </c>
-      <c r="G4" s="9">
-        <f>((D4-F4)/F4)</f>
-        <v>-0.12366681594267802</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>109492</v>
-      </c>
-      <c r="C5" s="2">
-        <v>103509</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3603865</v>
-      </c>
-      <c r="E5" s="3">
-        <v>252</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="11">
-        <f>F6*0.00027</f>
-        <v>2088.1799999999998</v>
-      </c>
-      <c r="F6" s="8">
-        <v>7734000</v>
-      </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11">
-        <f t="shared" ref="E7:E8" si="0">F7*0.00027</f>
-        <v>1256.04</v>
-      </c>
-      <c r="F7" s="8">
-        <v>4652000</v>
-      </c>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="11">
-        <f t="shared" si="0"/>
-        <v>116.37</v>
-      </c>
-      <c r="F8" s="8">
-        <v>431000</v>
-      </c>
-      <c r="G8" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567AE2A3-6B7B-4A00-9CB4-A51A259DF17A}">
   <dimension ref="D3:BG19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:AZ1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,196 +450,196 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:59" x14ac:dyDescent="0.25">
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="str">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="str">
         <f t="shared" ref="E3:H3" si="0">DEC2HEX(E11+E10*2+E9*4+E8*8+E7*16+E6*32+E5*64+E4*128)</f>
         <v>7C</v>
       </c>
-      <c r="F3" s="15" t="str">
+      <c r="F3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G3" s="15" t="str">
+      <c r="G3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H3" s="15" t="str">
+      <c r="H3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I3" s="15" t="str">
+      <c r="I3" s="1" t="str">
         <f>DEC2HEX(I11+I10*2+I9*4+I8*8+I7*16+I6*32+I5*64+I4*128)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="15" t="str">
+      <c r="J3" s="1" t="str">
         <f>DEC2HEX(J11+J10*2+J9*4+J8*8+J7*16+J6*32+J5*64+J4*128)</f>
         <v>14</v>
       </c>
-      <c r="K3" s="15" t="str">
+      <c r="K3" s="1" t="str">
         <f>DEC2HEX(K11+K10*2+K9*4+K8*8+K7*16+K6*32+K5*64+K4*128)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="15" t="str">
+      <c r="L3" s="1" t="str">
         <f>DEC2HEX(L11+L10*2+L9*4+L8*8+L7*16+L6*32+L5*64+L4*128)</f>
         <v>20</v>
       </c>
-      <c r="M3" s="15" t="str">
+      <c r="M3" s="1" t="str">
         <f t="shared" ref="M3:O3" si="1">DEC2HEX(M11+M10*2+M9*4+M8*8+M7*16+M6*32+M5*64+M4*128)</f>
         <v>40</v>
       </c>
-      <c r="N3" s="15" t="str">
+      <c r="N3" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FF</v>
       </c>
-      <c r="O3" s="15" t="str">
+      <c r="O3" s="1" t="str">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="P3" s="15" t="str">
+      <c r="P3" s="1" t="str">
         <f>DEC2HEX(P11+P10*2+P9*4+P8*8+P7*16+P6*32+P5*64+P4*128)</f>
         <v>20</v>
       </c>
-      <c r="Q3" s="15" t="str">
+      <c r="Q3" s="1" t="str">
         <f t="shared" ref="Q3:AZ3" si="2">DEC2HEX(Q11+Q10*2+Q9*4+Q8*8+Q7*16+Q6*32+Q5*64+Q4*128)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="15" t="str">
+      <c r="R3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S3" s="15" t="str">
+      <c r="S3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="T3" s="15" t="str">
+      <c r="T3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>3F</v>
       </c>
-      <c r="U3" s="15" t="str">
+      <c r="U3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="V3" s="15" t="str">
+      <c r="V3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="W3" s="15" t="str">
+      <c r="W3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X3" s="15" t="str">
+      <c r="X3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Y3" s="15" t="str">
+      <c r="Y3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Z3" s="15" t="str">
+      <c r="Z3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="AA3" s="15" t="str">
+      <c r="AA3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="AB3" s="15" t="str">
+      <c r="AB3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="AC3" s="15" t="str">
+      <c r="AC3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AD3" s="15" t="str">
+      <c r="AD3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="AE3" s="15" t="str">
+      <c r="AE3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="AF3" s="15" t="str">
+      <c r="AF3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="AG3" s="15" t="str">
+      <c r="AG3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="AH3" s="15" t="str">
+      <c r="AH3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="AI3" s="15" t="str">
+      <c r="AI3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ3" s="15" t="str">
+      <c r="AJ3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="AK3" s="15" t="str">
+      <c r="AK3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="AL3" s="15" t="str">
+      <c r="AL3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>F0</v>
       </c>
-      <c r="AM3" s="15" t="str">
+      <c r="AM3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="AN3" s="15" t="str">
+      <c r="AN3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="AO3" s="15" t="str">
+      <c r="AO3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AP3" s="15" t="str">
+      <c r="AP3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="AQ3" s="15" t="str">
+      <c r="AQ3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="AR3" s="15" t="str">
+      <c r="AR3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FC</v>
       </c>
-      <c r="AS3" s="15" t="str">
+      <c r="AS3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="AT3" s="15" t="str">
+      <c r="AT3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="AU3" s="15" t="str">
+      <c r="AU3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AV3" s="15" t="str">
+      <c r="AV3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="AW3" s="15" t="str">
+      <c r="AW3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="AX3" s="15" t="str">
+      <c r="AX3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FF</v>
       </c>
-      <c r="AY3" s="15" t="str">
+      <c r="AY3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="AZ3" s="15" t="str">
+      <c r="AZ3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
@@ -1173,91 +890,91 @@
       </c>
     </row>
     <row r="12" spans="4:59" x14ac:dyDescent="0.25">
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE12" s="16"/>
-      <c r="AF12" s="16"/>
-      <c r="AG12" s="16"/>
-      <c r="AH12" s="16"/>
-      <c r="AI12" s="16"/>
-      <c r="AJ12" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AK12" s="16"/>
-      <c r="AL12" s="16"/>
-      <c r="AM12" s="16"/>
-      <c r="AN12" s="16"/>
-      <c r="AO12" s="16"/>
-      <c r="AP12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="AQ12" s="16"/>
-      <c r="AR12" s="16"/>
-      <c r="AS12" s="16"/>
-      <c r="AT12" s="16"/>
-      <c r="AU12" s="16"/>
-      <c r="AV12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW12" s="16"/>
-      <c r="AX12" s="16"/>
-      <c r="AY12" s="16"/>
-      <c r="AZ12" s="16"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
     </row>
     <row r="13" spans="4:59" x14ac:dyDescent="0.25">
       <c r="L13" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="X13" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AD13" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AJ13" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="AP13" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="AV13" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="4:59" x14ac:dyDescent="0.25">
@@ -1459,4 +1176,948 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3860784D-6D69-4063-9766-5975109BDCD9}">
+  <dimension ref="B3:K73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="42" width="1.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="K3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(B3*128+C3*64+D3*32+E3*16+F3*8+G3*4+H3*2+I3),",  /*",IF(B3=0,"0","1"),IF(C3=0,"0","1"),IF(D3=0,"0","1"),IF(E3=0,"0","1"),IF(F3=0,"0","1"),IF(G3=0,"0","1"),"*/")</f>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K19" si="0">_xlfn.CONCAT("0x",DEC2HEX(B4*128+C4*64+D4*32+E4*16+F4*8+G4*4+H4*2+I4),",  /*",IF(B4=0,"0","1"),IF(C4=0,"0","1"),IF(D4=0,"0","1"),IF(E4=0,"0","1"),IF(F4=0,"0","1"),IF(G4=0,"0","1"),"*/")</f>
+        <v>0x38,  /*001110*/</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>0x54,  /*010101*/</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="K12" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(B12*128+C12*64+D12*32+E12*16+F12*8+G12*4+H12*2+I12),",  /*",IF(B12=0,"0","1"),IF(C12=0,"0","1"),IF(D12=0,"0","1"),IF(E12=0,"0","1"),IF(F12=0,"0","1"),IF(G12=0,"0","1"),"*/")</f>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>0x38,  /*001110*/</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>0x54,  /*010101*/</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="K21" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(B21*128+C21*64+D21*32+E21*16+F21*8+G21*4+H21*2+I21),",  /*",IF(B21=0,"0","1"),IF(C21=0,"0","1"),IF(D21=0,"0","1"),IF(E21=0,"0","1"),IF(F21=0,"0","1"),IF(G21=0,"0","1"),"*/")</f>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="K22" t="str">
+        <f t="shared" ref="K22:K28" si="1">_xlfn.CONCAT("0x",DEC2HEX(B22*128+C22*64+D22*32+E22*16+F22*8+G22*4+H22*2+I22),",  /*",IF(B22=0,"0","1"),IF(C22=0,"0","1"),IF(D22=0,"0","1"),IF(E22=0,"0","1"),IF(F22=0,"0","1"),IF(G22=0,"0","1"),"*/")</f>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>0x38,  /*001110*/</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>0x54,  /*010101*/</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="K30" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(B30*128+C30*64+D30*32+E30*16+F30*8+G30*4+H30*2+I30),",  /*",IF(B30=0,"0","1"),IF(C30=0,"0","1"),IF(D30=0,"0","1"),IF(E30=0,"0","1"),IF(F30=0,"0","1"),IF(G30=0,"0","1"),"*/")</f>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="K31" t="str">
+        <f t="shared" ref="K31:K37" si="2">_xlfn.CONCAT("0x",DEC2HEX(B31*128+C31*64+D31*32+E31*16+F31*8+G31*4+H31*2+I31),",  /*",IF(B31=0,"0","1"),IF(C31=0,"0","1"),IF(D31=0,"0","1"),IF(E31=0,"0","1"),IF(F31=0,"0","1"),IF(G31=0,"0","1"),"*/")</f>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="K32" t="str">
+        <f t="shared" si="2"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="K33" t="str">
+        <f t="shared" si="2"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="2"/>
+        <v>0x7C,  /*011111*/</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="K35" t="str">
+        <f t="shared" si="2"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="K36" t="str">
+        <f t="shared" si="2"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="K37" t="str">
+        <f t="shared" si="2"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3">
+        <v>1</v>
+      </c>
+      <c r="K39" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(B39*128+C39*64+D39*32+E39*16+F39*8+G39*4+H39*2+I39),",  /*",IF(B39=0,"0","1"),IF(C39=0,"0","1"),IF(D39=0,"0","1"),IF(E39=0,"0","1"),IF(F39=0,"0","1"),IF(G39=0,"0","1"),"*/")</f>
+        <v>0x54,  /*010101*/</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="K40" t="str">
+        <f t="shared" ref="K40:K46" si="3">_xlfn.CONCAT("0x",DEC2HEX(B40*128+C40*64+D40*32+E40*16+F40*8+G40*4+H40*2+I40),",  /*",IF(B40=0,"0","1"),IF(C40=0,"0","1"),IF(D40=0,"0","1"),IF(E40=0,"0","1"),IF(F40=0,"0","1"),IF(G40=0,"0","1"),"*/")</f>
+        <v>0x38,  /*001110*/</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="K41" t="str">
+        <f t="shared" si="3"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="K42" t="str">
+        <f t="shared" si="3"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="K43" t="str">
+        <f t="shared" si="3"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="K44" t="str">
+        <f t="shared" si="3"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="K45" t="str">
+        <f t="shared" si="3"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="K46" t="str">
+        <f t="shared" si="3"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="K48" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(B48*128+C48*64+D48*32+E48*16+F48*8+G48*4+H48*2+I48),",  /*",IF(B48=0,"0","1"),IF(C48=0,"0","1"),IF(D48=0,"0","1"),IF(E48=0,"0","1"),IF(F48=0,"0","1"),IF(G48=0,"0","1"),"*/")</f>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="K49" t="str">
+        <f t="shared" ref="K49:K55" si="4">_xlfn.CONCAT("0x",DEC2HEX(B49*128+C49*64+D49*32+E49*16+F49*8+G49*4+H49*2+I49),",  /*",IF(B49=0,"0","1"),IF(C49=0,"0","1"),IF(D49=0,"0","1"),IF(E49=0,"0","1"),IF(F49=0,"0","1"),IF(G49=0,"0","1"),"*/")</f>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3">
+        <v>1</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="4"/>
+        <v>0x54,  /*010101*/</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="K51" t="str">
+        <f t="shared" si="4"/>
+        <v>0x38,  /*001110*/</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="K52" t="str">
+        <f t="shared" si="4"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="K53" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="K54" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="K55" t="str">
+        <f t="shared" si="4"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="K57" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(B57*128+C57*64+D57*32+E57*16+F57*8+G57*4+H57*2+I57),",  /*",IF(B57=0,"0","1"),IF(C57=0,"0","1"),IF(D57=0,"0","1"),IF(E57=0,"0","1"),IF(F57=0,"0","1"),IF(G57=0,"0","1"),"*/")</f>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="K58" t="str">
+        <f t="shared" ref="K58:K64" si="5">_xlfn.CONCAT("0x",DEC2HEX(B58*128+C58*64+D58*32+E58*16+F58*8+G58*4+H58*2+I58),",  /*",IF(B58=0,"0","1"),IF(C58=0,"0","1"),IF(D58=0,"0","1"),IF(E58=0,"0","1"),IF(F58=0,"0","1"),IF(G58=0,"0","1"),"*/")</f>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="K59" t="str">
+        <f t="shared" si="5"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="K60" t="str">
+        <f t="shared" si="5"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3">
+        <v>1</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3">
+        <v>1</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="5"/>
+        <v>0x54,  /*010101*/</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3">
+        <v>1</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3"/>
+      <c r="K62" t="str">
+        <f t="shared" si="5"/>
+        <v>0x38,  /*001110*/</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="K63" t="str">
+        <f t="shared" si="5"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="K64" t="str">
+        <f t="shared" si="5"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+      <c r="C66" s="3">
+        <v>1</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="K66" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(B66*128+C66*64+D66*32+E66*16+F66*8+G66*4+H66*2+I66),",  /*",IF(B66=0,"0","1"),IF(C66=0,"0","1"),IF(D66=0,"0","1"),IF(E66=0,"0","1"),IF(F66=0,"0","1"),IF(G66=0,"0","1"),"*/")</f>
+        <v>0x40,  /*010000*/</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3">
+        <v>1</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K73" si="6">_xlfn.CONCAT("0x",DEC2HEX(B67*128+C67*64+D67*32+E67*16+F67*8+G67*4+H67*2+I67),",  /*",IF(B67=0,"0","1"),IF(C67=0,"0","1"),IF(D67=0,"0","1"),IF(E67=0,"0","1"),IF(F67=0,"0","1"),IF(G67=0,"0","1"),"*/")</f>
+        <v>0x28,  /*001010*/</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3">
+        <v>1</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3">
+        <v>1</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="6"/>
+        <v>0x54,  /*010101*/</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3">
+        <v>1</v>
+      </c>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3">
+        <v>1</v>
+      </c>
+      <c r="G69" s="3"/>
+      <c r="K69" t="str">
+        <f t="shared" si="6"/>
+        <v>0x28,  /*001010*/</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3">
+        <v>1</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3">
+        <v>1</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3">
+        <v>1</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="6"/>
+        <v>0x54,  /*010101*/</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
+      <c r="G71" s="3"/>
+      <c r="K71" t="str">
+        <f t="shared" si="6"/>
+        <v>0x28,  /*001010*/</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="K72" t="str">
+        <f t="shared" si="6"/>
+        <v>0x10,  /*000100*/</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="K73" t="str">
+        <f t="shared" si="6"/>
+        <v>0x0,  /*000000*/</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18720BB-280E-4991-8EAB-FB6A88053E47}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>